<commit_message>
Added new cases for tests
</commit_message>
<xml_diff>
--- a/XmlProcessingTeste/SoapUI Results.xlsx
+++ b/XmlProcessingTeste/SoapUI Results.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\source\repos\XmlProcessingTester\XmlProcessingTeste\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02E8D8BE-9AAE-483C-A1DB-977B2A75DF81}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3DE1A8A-8B57-4EE3-A034-84DFEE27AFC5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{CA9D6D52-75AD-48D1-AC7B-A000D2427B36}"/>
+    <workbookView xWindow="-120" yWindow="480" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{CA9D6D52-75AD-48D1-AC7B-A000D2427B36}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Doc vs. Reader" sheetId="2" r:id="rId2"/>
+    <sheet name="Doc vs. Reader WSH" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="499" uniqueCount="25">
   <si>
     <t>ProcessDocument</t>
   </si>
@@ -178,17 +179,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -515,19 +516,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+      <c r="A1" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
-      <c r="I1" s="4"/>
-      <c r="J1" s="4"/>
-      <c r="K1" s="4"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
+      <c r="G1" s="6"/>
+      <c r="H1" s="6"/>
+      <c r="I1" s="6"/>
+      <c r="J1" s="6"/>
+      <c r="K1" s="6"/>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
@@ -670,19 +671,19 @@
       </c>
     </row>
     <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="4" t="s">
+      <c r="A8" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
-      <c r="H8" s="4"/>
-      <c r="I8" s="4"/>
-      <c r="J8" s="4"/>
-      <c r="K8" s="4"/>
+      <c r="B8" s="6"/>
+      <c r="C8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
+      <c r="K8" s="6"/>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
@@ -838,19 +839,19 @@
       <c r="K13" s="1"/>
     </row>
     <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" s="4" t="s">
+      <c r="A15" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4"/>
-      <c r="C15" s="4"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
-      <c r="H15" s="4"/>
-      <c r="I15" s="4"/>
-      <c r="J15" s="4"/>
-      <c r="K15" s="4"/>
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
+      <c r="K15" s="6"/>
     </row>
     <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
@@ -993,19 +994,19 @@
       </c>
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" s="4" t="s">
+      <c r="A22" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B22" s="4"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
-      <c r="H22" s="4"/>
-      <c r="I22" s="4"/>
-      <c r="J22" s="4"/>
-      <c r="K22" s="4"/>
+      <c r="B22" s="6"/>
+      <c r="C22" s="6"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="6"/>
+      <c r="I22" s="6"/>
+      <c r="J22" s="6"/>
+      <c r="K22" s="6"/>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
@@ -1148,19 +1149,19 @@
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" s="4" t="s">
+      <c r="A29" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B29" s="4"/>
-      <c r="C29" s="4"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
-      <c r="H29" s="4"/>
-      <c r="I29" s="4"/>
-      <c r="J29" s="4"/>
-      <c r="K29" s="4"/>
+      <c r="B29" s="6"/>
+      <c r="C29" s="6"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="6"/>
+      <c r="F29" s="6"/>
+      <c r="G29" s="6"/>
+      <c r="H29" s="6"/>
+      <c r="I29" s="6"/>
+      <c r="J29" s="6"/>
+      <c r="K29" s="6"/>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
@@ -1303,19 +1304,19 @@
       </c>
     </row>
     <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" s="4" t="s">
+      <c r="A36" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="B36" s="4"/>
-      <c r="C36" s="4"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
-      <c r="H36" s="4"/>
-      <c r="I36" s="4"/>
-      <c r="J36" s="4"/>
-      <c r="K36" s="4"/>
+      <c r="B36" s="6"/>
+      <c r="C36" s="6"/>
+      <c r="D36" s="6"/>
+      <c r="E36" s="6"/>
+      <c r="F36" s="6"/>
+      <c r="G36" s="6"/>
+      <c r="H36" s="6"/>
+      <c r="I36" s="6"/>
+      <c r="J36" s="6"/>
+      <c r="K36" s="6"/>
     </row>
     <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
@@ -1458,19 +1459,19 @@
       </c>
     </row>
     <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" s="4" t="s">
+      <c r="A43" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
-      <c r="H43" s="4"/>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
+      <c r="B43" s="6"/>
+      <c r="C43" s="6"/>
+      <c r="D43" s="6"/>
+      <c r="E43" s="6"/>
+      <c r="F43" s="6"/>
+      <c r="G43" s="6"/>
+      <c r="H43" s="6"/>
+      <c r="I43" s="6"/>
+      <c r="J43" s="6"/>
+      <c r="K43" s="6"/>
     </row>
     <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
@@ -1613,19 +1614,19 @@
       </c>
     </row>
     <row r="50" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A50" s="4" t="s">
+      <c r="A50" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B50" s="4"/>
-      <c r="C50" s="4"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="4"/>
-      <c r="I50" s="4"/>
-      <c r="J50" s="4"/>
-      <c r="K50" s="4"/>
+      <c r="B50" s="6"/>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6"/>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="6"/>
+      <c r="H50" s="6"/>
+      <c r="I50" s="6"/>
+      <c r="J50" s="6"/>
+      <c r="K50" s="6"/>
     </row>
     <row r="51" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
@@ -1768,19 +1769,19 @@
       </c>
     </row>
     <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" s="4" t="s">
+      <c r="A57" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B57" s="4"/>
-      <c r="C57" s="4"/>
-      <c r="D57" s="4"/>
-      <c r="E57" s="4"/>
-      <c r="F57" s="4"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="4"/>
-      <c r="I57" s="4"/>
-      <c r="J57" s="4"/>
-      <c r="K57" s="4"/>
+      <c r="B57" s="6"/>
+      <c r="C57" s="6"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="6"/>
+      <c r="F57" s="6"/>
+      <c r="G57" s="6"/>
+      <c r="H57" s="6"/>
+      <c r="I57" s="6"/>
+      <c r="J57" s="6"/>
+      <c r="K57" s="6"/>
     </row>
     <row r="58" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
@@ -1923,19 +1924,19 @@
       </c>
     </row>
     <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" s="4" t="s">
+      <c r="A64" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B64" s="4"/>
-      <c r="C64" s="4"/>
-      <c r="D64" s="4"/>
-      <c r="E64" s="4"/>
-      <c r="F64" s="4"/>
-      <c r="G64" s="4"/>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4"/>
-      <c r="J64" s="4"/>
-      <c r="K64" s="4"/>
+      <c r="B64" s="6"/>
+      <c r="C64" s="6"/>
+      <c r="D64" s="6"/>
+      <c r="E64" s="6"/>
+      <c r="F64" s="6"/>
+      <c r="G64" s="6"/>
+      <c r="H64" s="6"/>
+      <c r="I64" s="6"/>
+      <c r="J64" s="6"/>
+      <c r="K64" s="6"/>
     </row>
     <row r="65" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
@@ -2078,19 +2079,19 @@
       </c>
     </row>
     <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" s="4" t="s">
+      <c r="A71" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B71" s="4"/>
-      <c r="C71" s="4"/>
-      <c r="D71" s="4"/>
-      <c r="E71" s="4"/>
-      <c r="F71" s="4"/>
-      <c r="G71" s="4"/>
-      <c r="H71" s="4"/>
-      <c r="I71" s="4"/>
-      <c r="J71" s="4"/>
-      <c r="K71" s="4"/>
+      <c r="B71" s="6"/>
+      <c r="C71" s="6"/>
+      <c r="D71" s="6"/>
+      <c r="E71" s="6"/>
+      <c r="F71" s="6"/>
+      <c r="G71" s="6"/>
+      <c r="H71" s="6"/>
+      <c r="I71" s="6"/>
+      <c r="J71" s="6"/>
+      <c r="K71" s="6"/>
     </row>
     <row r="72" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
@@ -2233,19 +2234,19 @@
       </c>
     </row>
     <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" s="4" t="s">
+      <c r="A78" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B78" s="4"/>
-      <c r="C78" s="4"/>
-      <c r="D78" s="4"/>
-      <c r="E78" s="4"/>
-      <c r="F78" s="4"/>
-      <c r="G78" s="4"/>
-      <c r="H78" s="4"/>
-      <c r="I78" s="4"/>
-      <c r="J78" s="4"/>
-      <c r="K78" s="4"/>
+      <c r="B78" s="6"/>
+      <c r="C78" s="6"/>
+      <c r="D78" s="6"/>
+      <c r="E78" s="6"/>
+      <c r="F78" s="6"/>
+      <c r="G78" s="6"/>
+      <c r="H78" s="6"/>
+      <c r="I78" s="6"/>
+      <c r="J78" s="6"/>
+      <c r="K78" s="6"/>
     </row>
     <row r="79" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
@@ -2388,19 +2389,19 @@
       </c>
     </row>
     <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" s="4" t="s">
+      <c r="A85" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="B85" s="4"/>
-      <c r="C85" s="4"/>
-      <c r="D85" s="4"/>
-      <c r="E85" s="4"/>
-      <c r="F85" s="4"/>
-      <c r="G85" s="4"/>
-      <c r="H85" s="4"/>
-      <c r="I85" s="4"/>
-      <c r="J85" s="4"/>
-      <c r="K85" s="4"/>
+      <c r="B85" s="6"/>
+      <c r="C85" s="6"/>
+      <c r="D85" s="6"/>
+      <c r="E85" s="6"/>
+      <c r="F85" s="6"/>
+      <c r="G85" s="6"/>
+      <c r="H85" s="6"/>
+      <c r="I85" s="6"/>
+      <c r="J85" s="6"/>
+      <c r="K85" s="6"/>
     </row>
     <row r="86" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
@@ -2544,6 +2545,12 @@
     </row>
   </sheetData>
   <mergeCells count="13">
+    <mergeCell ref="A36:K36"/>
+    <mergeCell ref="A1:K1"/>
+    <mergeCell ref="A8:K8"/>
+    <mergeCell ref="A15:K15"/>
+    <mergeCell ref="A22:K22"/>
+    <mergeCell ref="A29:K29"/>
     <mergeCell ref="A85:K85"/>
     <mergeCell ref="A43:K43"/>
     <mergeCell ref="A50:K50"/>
@@ -2551,12 +2558,6 @@
     <mergeCell ref="A64:K64"/>
     <mergeCell ref="A71:K71"/>
     <mergeCell ref="A78:K78"/>
-    <mergeCell ref="A36:K36"/>
-    <mergeCell ref="A1:K1"/>
-    <mergeCell ref="A8:K8"/>
-    <mergeCell ref="A15:K15"/>
-    <mergeCell ref="A22:K22"/>
-    <mergeCell ref="A29:K29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -2566,7 +2567,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7D292DA2-7F91-4FCF-B69D-1918C451F562}">
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N32" sqref="N32"/>
     </sheetView>
   </sheetViews>
@@ -2577,20 +2578,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A1" s="5" t="s">
+      <c r="A1" s="8" t="s">
         <v>23</v>
       </c>
-      <c r="B1" s="5"/>
-      <c r="C1" s="5"/>
-      <c r="D1" s="5"/>
-      <c r="E1" s="5"/>
-      <c r="F1" s="5"/>
-      <c r="G1" s="5"/>
-      <c r="H1" s="5"/>
-      <c r="I1" s="5"/>
-      <c r="J1" s="5"/>
-      <c r="K1" s="5"/>
-      <c r="L1" s="5"/>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
       <c r="O1" s="7" t="s">
         <v>24</v>
       </c>
@@ -2607,20 +2608,20 @@
       <c r="Z1" s="7"/>
     </row>
     <row r="2" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A2" s="5" t="s">
+      <c r="A2" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="5"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
       <c r="O2" s="7" t="s">
         <v>14</v>
       </c>
@@ -2637,76 +2638,76 @@
       <c r="Z2" s="7"/>
     </row>
     <row r="3" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
+      <c r="A3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C3" s="6" t="s">
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D3" s="6" t="s">
+      <c r="D3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F3" s="6" t="s">
+      <c r="F3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G3" s="6" t="s">
+      <c r="G3" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="6" t="s">
+      <c r="H3" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L3" s="6" t="s">
+      <c r="L3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O3" s="8" t="s">
+      <c r="O3" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P3" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q3" s="8" t="s">
+      <c r="P3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="R3" s="8" t="s">
+      <c r="R3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="S3" s="8" t="s">
+      <c r="S3" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="T3" s="8" t="s">
+      <c r="T3" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="U3" s="8" t="s">
+      <c r="U3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="V3" s="8" t="s">
+      <c r="V3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="W3" s="8" t="s">
+      <c r="W3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="X3" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Y3" s="8" t="s">
+      <c r="Y3" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Z3" s="8" t="s">
+      <c r="Z3" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -3599,20 +3600,20 @@
       </c>
     </row>
     <row r="17" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A17" s="5" t="s">
+      <c r="A17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="B17" s="5"/>
-      <c r="C17" s="5"/>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
-      <c r="K17" s="5"/>
-      <c r="L17" s="5"/>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
       <c r="O17" s="7" t="s">
         <v>21</v>
       </c>
@@ -3629,76 +3630,76 @@
       <c r="Z17" s="7"/>
     </row>
     <row r="18" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A18" s="6" t="s">
+      <c r="A18" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B18" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C18" s="6" t="s">
+      <c r="B18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D18" s="6" t="s">
+      <c r="D18" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E18" s="6" t="s">
+      <c r="E18" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="6" t="s">
+      <c r="F18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="6" t="s">
+      <c r="G18" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H18" s="6" t="s">
+      <c r="H18" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I18" s="6" t="s">
+      <c r="I18" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J18" s="6" t="s">
+      <c r="J18" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K18" s="6" t="s">
+      <c r="K18" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L18" s="6" t="s">
+      <c r="L18" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O18" s="8" t="s">
+      <c r="O18" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P18" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q18" s="8" t="s">
+      <c r="P18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="R18" s="8" t="s">
+      <c r="R18" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="S18" s="8" t="s">
+      <c r="S18" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="T18" s="8" t="s">
+      <c r="T18" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="U18" s="8" t="s">
+      <c r="U18" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="V18" s="8" t="s">
+      <c r="V18" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="W18" s="8" t="s">
+      <c r="W18" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="X18" s="8" t="s">
+      <c r="X18" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Y18" s="8" t="s">
+      <c r="Y18" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Z18" s="8" t="s">
+      <c r="Z18" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -4591,20 +4592,20 @@
       </c>
     </row>
     <row r="33" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A33" s="5" t="s">
+      <c r="A33" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="B33" s="5"/>
-      <c r="C33" s="5"/>
-      <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
-      <c r="F33" s="5"/>
-      <c r="G33" s="5"/>
-      <c r="H33" s="5"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="5"/>
-      <c r="K33" s="5"/>
-      <c r="L33" s="5"/>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
       <c r="O33" s="7" t="s">
         <v>22</v>
       </c>
@@ -4621,76 +4622,76 @@
       <c r="Z33" s="7"/>
     </row>
     <row r="34" spans="1:26" x14ac:dyDescent="0.25">
-      <c r="A34" s="6" t="s">
+      <c r="A34" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B34" s="6" t="s">
-        <v>3</v>
-      </c>
-      <c r="C34" s="6" t="s">
+      <c r="B34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D34" s="6" t="s">
+      <c r="D34" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E34" s="6" t="s">
+      <c r="E34" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="6" t="s">
+      <c r="F34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="G34" s="6" t="s">
+      <c r="G34" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H34" s="6" t="s">
+      <c r="H34" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="I34" s="6" t="s">
+      <c r="I34" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="J34" s="6" t="s">
+      <c r="J34" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="K34" s="6" t="s">
+      <c r="K34" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="L34" s="6" t="s">
+      <c r="L34" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="O34" s="8" t="s">
+      <c r="O34" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="P34" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q34" s="8" t="s">
+      <c r="P34" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q34" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="R34" s="8" t="s">
+      <c r="R34" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="S34" s="8" t="s">
+      <c r="S34" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="T34" s="8" t="s">
+      <c r="T34" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="U34" s="8" t="s">
+      <c r="U34" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="V34" s="8" t="s">
+      <c r="V34" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="W34" s="8" t="s">
+      <c r="W34" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="X34" s="8" t="s">
+      <c r="X34" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="Y34" s="8" t="s">
+      <c r="Y34" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="Z34" s="8" t="s">
+      <c r="Z34" s="5" t="s">
         <v>13</v>
       </c>
     </row>
@@ -5595,4 +5596,3041 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8D2CF7D9-49DA-4865-B7D0-0AE6011DD963}">
+  <dimension ref="A1:Z46"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A22" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="T41" sqref="T41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="14.7109375" customWidth="1"/>
+    <col min="9" max="9" width="15" customWidth="1"/>
+    <col min="16" max="16" width="14" customWidth="1"/>
+    <col min="23" max="23" width="16.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A1" s="8" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="8"/>
+      <c r="C1" s="8"/>
+      <c r="D1" s="8"/>
+      <c r="E1" s="8"/>
+      <c r="F1" s="8"/>
+      <c r="G1" s="8"/>
+      <c r="H1" s="8"/>
+      <c r="I1" s="8"/>
+      <c r="J1" s="8"/>
+      <c r="K1" s="8"/>
+      <c r="L1" s="8"/>
+      <c r="O1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="P1" s="7"/>
+      <c r="Q1" s="7"/>
+      <c r="R1" s="7"/>
+      <c r="S1" s="7"/>
+      <c r="T1" s="7"/>
+      <c r="U1" s="7"/>
+      <c r="V1" s="7"/>
+      <c r="W1" s="7"/>
+      <c r="X1" s="7"/>
+      <c r="Y1" s="7"/>
+      <c r="Z1" s="7"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A2" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B2" s="8"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="8"/>
+      <c r="G2" s="8"/>
+      <c r="H2" s="8"/>
+      <c r="I2" s="8"/>
+      <c r="J2" s="8"/>
+      <c r="K2" s="8"/>
+      <c r="L2" s="8"/>
+      <c r="O2" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="P2" s="7"/>
+      <c r="Q2" s="7"/>
+      <c r="R2" s="7"/>
+      <c r="S2" s="7"/>
+      <c r="T2" s="7"/>
+      <c r="U2" s="7"/>
+      <c r="V2" s="7"/>
+      <c r="W2" s="7"/>
+      <c r="X2" s="7"/>
+      <c r="Y2" s="7"/>
+      <c r="Z2" s="7"/>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H3" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J3" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K3" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L3" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q3" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S3" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="U3" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="V3" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="W3" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="X3" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y3" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z3" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
+        <v>1</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3">
+        <v>3.88</v>
+      </c>
+      <c r="F4" s="3">
+        <v>7</v>
+      </c>
+      <c r="G4" s="3">
+        <v>126</v>
+      </c>
+      <c r="H4" s="3">
+        <v>12.52</v>
+      </c>
+      <c r="I4" s="3">
+        <v>55419</v>
+      </c>
+      <c r="J4" s="3">
+        <v>5508</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0</v>
+      </c>
+      <c r="L4" s="3">
+        <v>0</v>
+      </c>
+      <c r="O4" s="3">
+        <v>1</v>
+      </c>
+      <c r="P4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" s="3">
+        <v>2</v>
+      </c>
+      <c r="R4" s="3">
+        <v>16</v>
+      </c>
+      <c r="S4" s="3">
+        <v>3.08</v>
+      </c>
+      <c r="T4" s="3">
+        <v>3</v>
+      </c>
+      <c r="U4" s="3">
+        <v>125</v>
+      </c>
+      <c r="V4" s="3">
+        <v>12.43</v>
+      </c>
+      <c r="W4" s="3">
+        <v>337964</v>
+      </c>
+      <c r="X4" s="3">
+        <v>33618</v>
+      </c>
+      <c r="Y4" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z4" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
+        <v>2</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3">
+        <v>35</v>
+      </c>
+      <c r="E5" s="3">
+        <v>4.5199999999999996</v>
+      </c>
+      <c r="F5" s="3">
+        <v>3</v>
+      </c>
+      <c r="G5" s="3">
+        <v>128</v>
+      </c>
+      <c r="H5" s="3">
+        <v>12.72</v>
+      </c>
+      <c r="I5" s="3">
+        <v>56291</v>
+      </c>
+      <c r="J5" s="3">
+        <v>5596</v>
+      </c>
+      <c r="K5" s="3">
+        <v>0</v>
+      </c>
+      <c r="L5" s="3">
+        <v>0</v>
+      </c>
+      <c r="O5" s="3">
+        <v>2</v>
+      </c>
+      <c r="P5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q5" s="3">
+        <v>2</v>
+      </c>
+      <c r="R5" s="3">
+        <v>60</v>
+      </c>
+      <c r="S5" s="3">
+        <v>4.62</v>
+      </c>
+      <c r="T5" s="3">
+        <v>3</v>
+      </c>
+      <c r="U5" s="3">
+        <v>129</v>
+      </c>
+      <c r="V5" s="3">
+        <v>12.78</v>
+      </c>
+      <c r="W5" s="3">
+        <v>348786</v>
+      </c>
+      <c r="X5" s="3">
+        <v>34564</v>
+      </c>
+      <c r="Y5" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
+        <v>3</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C6" s="3">
+        <v>2</v>
+      </c>
+      <c r="D6" s="3">
+        <v>43</v>
+      </c>
+      <c r="E6" s="3">
+        <v>5.39</v>
+      </c>
+      <c r="F6" s="3">
+        <v>3</v>
+      </c>
+      <c r="G6" s="3">
+        <v>130</v>
+      </c>
+      <c r="H6" s="3">
+        <v>12.73</v>
+      </c>
+      <c r="I6" s="3">
+        <v>57168</v>
+      </c>
+      <c r="J6" s="3">
+        <v>5601</v>
+      </c>
+      <c r="K6" s="3">
+        <v>0</v>
+      </c>
+      <c r="L6" s="3">
+        <v>0</v>
+      </c>
+      <c r="O6" s="3">
+        <v>3</v>
+      </c>
+      <c r="P6" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q6" s="3">
+        <v>2</v>
+      </c>
+      <c r="R6" s="3">
+        <v>22</v>
+      </c>
+      <c r="S6" s="3">
+        <v>3.57</v>
+      </c>
+      <c r="T6" s="3">
+        <v>3</v>
+      </c>
+      <c r="U6" s="3">
+        <v>132</v>
+      </c>
+      <c r="V6" s="3">
+        <v>13.12</v>
+      </c>
+      <c r="W6" s="3">
+        <v>356897</v>
+      </c>
+      <c r="X6" s="3">
+        <v>35480</v>
+      </c>
+      <c r="Y6" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
+        <v>4</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3">
+        <v>2</v>
+      </c>
+      <c r="D7" s="3">
+        <v>126</v>
+      </c>
+      <c r="E7" s="3">
+        <v>6.85</v>
+      </c>
+      <c r="F7" s="3">
+        <v>3</v>
+      </c>
+      <c r="G7" s="3">
+        <v>128</v>
+      </c>
+      <c r="H7" s="3">
+        <v>12.54</v>
+      </c>
+      <c r="I7" s="3">
+        <v>56288</v>
+      </c>
+      <c r="J7" s="3">
+        <v>5517</v>
+      </c>
+      <c r="K7" s="3">
+        <v>0</v>
+      </c>
+      <c r="L7" s="3">
+        <v>0</v>
+      </c>
+      <c r="O7" s="3">
+        <v>4</v>
+      </c>
+      <c r="P7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q7" s="3">
+        <v>2</v>
+      </c>
+      <c r="R7" s="3">
+        <v>15</v>
+      </c>
+      <c r="S7" s="3">
+        <v>3.23</v>
+      </c>
+      <c r="T7" s="3">
+        <v>3</v>
+      </c>
+      <c r="U7" s="3">
+        <v>131</v>
+      </c>
+      <c r="V7" s="3">
+        <v>12.96</v>
+      </c>
+      <c r="W7" s="3">
+        <v>354192</v>
+      </c>
+      <c r="X7" s="3">
+        <v>35047</v>
+      </c>
+      <c r="Y7" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
+        <v>5</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C8" s="3">
+        <v>2</v>
+      </c>
+      <c r="D8" s="3">
+        <v>36</v>
+      </c>
+      <c r="E8" s="3">
+        <v>4.9400000000000004</v>
+      </c>
+      <c r="F8" s="3">
+        <v>4</v>
+      </c>
+      <c r="G8" s="3">
+        <v>131</v>
+      </c>
+      <c r="H8" s="3">
+        <v>12.71</v>
+      </c>
+      <c r="I8" s="3">
+        <v>57609</v>
+      </c>
+      <c r="J8" s="3">
+        <v>5589</v>
+      </c>
+      <c r="K8" s="3">
+        <v>0</v>
+      </c>
+      <c r="L8" s="3">
+        <v>0</v>
+      </c>
+      <c r="O8" s="3">
+        <v>5</v>
+      </c>
+      <c r="P8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q8" s="3">
+        <v>2</v>
+      </c>
+      <c r="R8" s="3">
+        <v>26</v>
+      </c>
+      <c r="S8" s="3">
+        <v>3.84</v>
+      </c>
+      <c r="T8" s="3">
+        <v>3</v>
+      </c>
+      <c r="U8" s="3">
+        <v>130</v>
+      </c>
+      <c r="V8" s="3">
+        <v>12.94</v>
+      </c>
+      <c r="W8" s="3">
+        <v>351494</v>
+      </c>
+      <c r="X8" s="3">
+        <v>35012</v>
+      </c>
+      <c r="Y8" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
+        <v>6</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" s="3">
+        <v>2</v>
+      </c>
+      <c r="D9" s="3">
+        <v>73</v>
+      </c>
+      <c r="E9" s="3">
+        <v>6.42</v>
+      </c>
+      <c r="F9" s="3">
+        <v>3</v>
+      </c>
+      <c r="G9" s="3">
+        <v>130</v>
+      </c>
+      <c r="H9" s="3">
+        <v>12.78</v>
+      </c>
+      <c r="I9" s="3">
+        <v>57171</v>
+      </c>
+      <c r="J9" s="3">
+        <v>5622</v>
+      </c>
+      <c r="K9" s="3">
+        <v>0</v>
+      </c>
+      <c r="L9" s="3">
+        <v>0</v>
+      </c>
+      <c r="O9" s="3">
+        <v>6</v>
+      </c>
+      <c r="P9" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q9" s="3">
+        <v>2</v>
+      </c>
+      <c r="R9" s="3">
+        <v>33</v>
+      </c>
+      <c r="S9" s="3">
+        <v>4.28</v>
+      </c>
+      <c r="T9" s="3">
+        <v>2</v>
+      </c>
+      <c r="U9" s="3">
+        <v>132</v>
+      </c>
+      <c r="V9" s="3">
+        <v>13.08</v>
+      </c>
+      <c r="W9" s="3">
+        <v>356906</v>
+      </c>
+      <c r="X9" s="3">
+        <v>35379</v>
+      </c>
+      <c r="Y9" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A10" s="3">
+        <v>7</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="3">
+        <v>2</v>
+      </c>
+      <c r="D10" s="3">
+        <v>40</v>
+      </c>
+      <c r="E10" s="3">
+        <v>4.84</v>
+      </c>
+      <c r="F10" s="3">
+        <v>4</v>
+      </c>
+      <c r="G10" s="3">
+        <v>129</v>
+      </c>
+      <c r="H10" s="3">
+        <v>12.58</v>
+      </c>
+      <c r="I10" s="3">
+        <v>56743</v>
+      </c>
+      <c r="J10" s="3">
+        <v>5536</v>
+      </c>
+      <c r="K10" s="3">
+        <v>0</v>
+      </c>
+      <c r="L10" s="3">
+        <v>0</v>
+      </c>
+      <c r="O10" s="3">
+        <v>7</v>
+      </c>
+      <c r="P10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q10" s="3">
+        <v>2</v>
+      </c>
+      <c r="R10" s="3">
+        <v>30</v>
+      </c>
+      <c r="S10" s="3">
+        <v>3.21</v>
+      </c>
+      <c r="T10" s="3">
+        <v>3</v>
+      </c>
+      <c r="U10" s="3">
+        <v>129</v>
+      </c>
+      <c r="V10" s="3">
+        <v>12.66</v>
+      </c>
+      <c r="W10" s="3">
+        <v>348786</v>
+      </c>
+      <c r="X10" s="3">
+        <v>34231</v>
+      </c>
+      <c r="Y10" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A11" s="3">
+        <v>8</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C11" s="3">
+        <v>2</v>
+      </c>
+      <c r="D11" s="3">
+        <v>101</v>
+      </c>
+      <c r="E11" s="3">
+        <v>8.1199999999999992</v>
+      </c>
+      <c r="F11" s="3">
+        <v>3</v>
+      </c>
+      <c r="G11" s="3">
+        <v>127</v>
+      </c>
+      <c r="H11" s="3">
+        <v>12.63</v>
+      </c>
+      <c r="I11" s="3">
+        <v>55861</v>
+      </c>
+      <c r="J11" s="3">
+        <v>5558</v>
+      </c>
+      <c r="K11" s="3">
+        <v>0</v>
+      </c>
+      <c r="L11" s="3">
+        <v>0</v>
+      </c>
+      <c r="O11" s="3">
+        <v>8</v>
+      </c>
+      <c r="P11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q11" s="3">
+        <v>2</v>
+      </c>
+      <c r="R11" s="3">
+        <v>84</v>
+      </c>
+      <c r="S11" s="3">
+        <v>4.16</v>
+      </c>
+      <c r="T11" s="3">
+        <v>3</v>
+      </c>
+      <c r="U11" s="3">
+        <v>127</v>
+      </c>
+      <c r="V11" s="3">
+        <v>12.45</v>
+      </c>
+      <c r="W11" s="3">
+        <v>343381</v>
+      </c>
+      <c r="X11" s="3">
+        <v>33671</v>
+      </c>
+      <c r="Y11" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A12" s="3">
+        <v>9</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C12" s="3">
+        <v>2</v>
+      </c>
+      <c r="D12" s="3">
+        <v>70</v>
+      </c>
+      <c r="E12" s="3">
+        <v>6.04</v>
+      </c>
+      <c r="F12" s="3">
+        <v>3</v>
+      </c>
+      <c r="G12" s="3">
+        <v>127</v>
+      </c>
+      <c r="H12" s="3">
+        <v>12.56</v>
+      </c>
+      <c r="I12" s="3">
+        <v>55855</v>
+      </c>
+      <c r="J12" s="3">
+        <v>5524</v>
+      </c>
+      <c r="K12" s="3">
+        <v>0</v>
+      </c>
+      <c r="L12" s="3">
+        <v>0</v>
+      </c>
+      <c r="O12" s="3">
+        <v>9</v>
+      </c>
+      <c r="P12" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q12" s="3">
+        <v>2</v>
+      </c>
+      <c r="R12" s="3">
+        <v>28</v>
+      </c>
+      <c r="S12" s="3">
+        <v>3.9</v>
+      </c>
+      <c r="T12" s="3">
+        <v>2</v>
+      </c>
+      <c r="U12" s="3">
+        <v>130</v>
+      </c>
+      <c r="V12" s="3">
+        <v>12.83</v>
+      </c>
+      <c r="W12" s="3">
+        <v>351483</v>
+      </c>
+      <c r="X12" s="3">
+        <v>34710</v>
+      </c>
+      <c r="Y12" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A13" s="3">
+        <v>10</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C13" s="3">
+        <v>2</v>
+      </c>
+      <c r="D13" s="3">
+        <v>65</v>
+      </c>
+      <c r="E13" s="3">
+        <v>6.07</v>
+      </c>
+      <c r="F13" s="3">
+        <v>3</v>
+      </c>
+      <c r="G13" s="3">
+        <v>126</v>
+      </c>
+      <c r="H13" s="3">
+        <v>12.51</v>
+      </c>
+      <c r="I13" s="3">
+        <v>55411</v>
+      </c>
+      <c r="J13" s="3">
+        <v>5505</v>
+      </c>
+      <c r="K13" s="3">
+        <v>0</v>
+      </c>
+      <c r="L13" s="3">
+        <v>0</v>
+      </c>
+      <c r="O13" s="3">
+        <v>10</v>
+      </c>
+      <c r="P13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q13" s="3">
+        <v>2</v>
+      </c>
+      <c r="R13" s="3">
+        <v>34</v>
+      </c>
+      <c r="S13" s="3">
+        <v>3.96</v>
+      </c>
+      <c r="T13" s="3">
+        <v>3</v>
+      </c>
+      <c r="U13" s="3">
+        <v>131</v>
+      </c>
+      <c r="V13" s="3">
+        <v>12.94</v>
+      </c>
+      <c r="W13" s="3">
+        <v>354199</v>
+      </c>
+      <c r="X13" s="3">
+        <v>35010</v>
+      </c>
+      <c r="Y13" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A14" s="3">
+        <v>11</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C14" s="3">
+        <v>2</v>
+      </c>
+      <c r="D14" s="3">
+        <v>84</v>
+      </c>
+      <c r="E14" s="3">
+        <v>8.5299999999999994</v>
+      </c>
+      <c r="F14" s="3">
+        <v>2</v>
+      </c>
+      <c r="G14" s="3">
+        <v>130</v>
+      </c>
+      <c r="H14" s="3">
+        <v>12.92</v>
+      </c>
+      <c r="I14" s="3">
+        <v>57168</v>
+      </c>
+      <c r="J14" s="3">
+        <v>5682</v>
+      </c>
+      <c r="K14" s="3">
+        <v>0</v>
+      </c>
+      <c r="L14" s="3">
+        <v>0</v>
+      </c>
+      <c r="O14" s="3">
+        <v>11</v>
+      </c>
+      <c r="P14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q14" s="3">
+        <v>2</v>
+      </c>
+      <c r="R14" s="3">
+        <v>11</v>
+      </c>
+      <c r="S14" s="3">
+        <v>2.99</v>
+      </c>
+      <c r="T14" s="3">
+        <v>2</v>
+      </c>
+      <c r="U14" s="3">
+        <v>134</v>
+      </c>
+      <c r="V14" s="3">
+        <v>13.31</v>
+      </c>
+      <c r="W14" s="3">
+        <v>362307</v>
+      </c>
+      <c r="X14" s="3">
+        <v>36003</v>
+      </c>
+      <c r="Y14" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A15" s="3">
+        <v>12</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C15" s="3">
+        <v>2</v>
+      </c>
+      <c r="D15" s="3">
+        <v>49</v>
+      </c>
+      <c r="E15" s="3">
+        <v>6.11</v>
+      </c>
+      <c r="F15" s="3">
+        <v>2</v>
+      </c>
+      <c r="G15" s="3">
+        <v>124</v>
+      </c>
+      <c r="H15" s="3">
+        <v>12.24</v>
+      </c>
+      <c r="I15" s="3">
+        <v>54531</v>
+      </c>
+      <c r="J15" s="3">
+        <v>5386</v>
+      </c>
+      <c r="K15" s="3">
+        <v>0</v>
+      </c>
+      <c r="L15" s="3">
+        <v>0</v>
+      </c>
+      <c r="O15" s="3">
+        <v>12</v>
+      </c>
+      <c r="P15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q15" s="3">
+        <v>2</v>
+      </c>
+      <c r="R15" s="3">
+        <v>12</v>
+      </c>
+      <c r="S15" s="3">
+        <v>3.3</v>
+      </c>
+      <c r="T15" s="3">
+        <v>4</v>
+      </c>
+      <c r="U15" s="3">
+        <v>130</v>
+      </c>
+      <c r="V15" s="3">
+        <v>12.8</v>
+      </c>
+      <c r="W15" s="3">
+        <v>351486</v>
+      </c>
+      <c r="X15" s="3">
+        <v>34615</v>
+      </c>
+      <c r="Y15" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" s="8"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="8"/>
+      <c r="I17" s="8"/>
+      <c r="J17" s="8"/>
+      <c r="K17" s="8"/>
+      <c r="L17" s="8"/>
+      <c r="O17" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+    </row>
+    <row r="18" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A18" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K18" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L18" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O18" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="P18" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q18" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S18" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T18" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="U18" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="V18" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="W18" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="X18" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y18" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z18" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C19" s="3">
+        <v>2</v>
+      </c>
+      <c r="D19" s="3">
+        <v>91</v>
+      </c>
+      <c r="E19" s="3">
+        <v>7.07</v>
+      </c>
+      <c r="F19" s="3">
+        <v>2</v>
+      </c>
+      <c r="G19" s="3">
+        <v>638</v>
+      </c>
+      <c r="H19" s="3">
+        <v>63.04</v>
+      </c>
+      <c r="I19" s="3">
+        <v>280569</v>
+      </c>
+      <c r="J19" s="3">
+        <v>27726</v>
+      </c>
+      <c r="K19" s="3">
+        <v>0</v>
+      </c>
+      <c r="L19" s="3">
+        <v>0</v>
+      </c>
+      <c r="O19" s="3">
+        <v>1</v>
+      </c>
+      <c r="P19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q19" s="3">
+        <v>2</v>
+      </c>
+      <c r="R19" s="3">
+        <v>63</v>
+      </c>
+      <c r="S19" s="3">
+        <v>4.58</v>
+      </c>
+      <c r="T19" s="3">
+        <v>16</v>
+      </c>
+      <c r="U19" s="3">
+        <v>633</v>
+      </c>
+      <c r="V19" s="3">
+        <v>62.61</v>
+      </c>
+      <c r="W19" s="3">
+        <v>1711481</v>
+      </c>
+      <c r="X19" s="3">
+        <v>169302</v>
+      </c>
+      <c r="Y19" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A20" s="3">
+        <v>2</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="3">
+        <v>2</v>
+      </c>
+      <c r="D20" s="3">
+        <v>283</v>
+      </c>
+      <c r="E20" s="3">
+        <v>13.14</v>
+      </c>
+      <c r="F20" s="3">
+        <v>31</v>
+      </c>
+      <c r="G20" s="3">
+        <v>632</v>
+      </c>
+      <c r="H20" s="3">
+        <v>62.81</v>
+      </c>
+      <c r="I20" s="3">
+        <v>277955</v>
+      </c>
+      <c r="J20" s="3">
+        <v>27626</v>
+      </c>
+      <c r="K20" s="3">
+        <v>0</v>
+      </c>
+      <c r="L20" s="3">
+        <v>0</v>
+      </c>
+      <c r="O20" s="3">
+        <v>2</v>
+      </c>
+      <c r="P20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q20" s="3">
+        <v>2</v>
+      </c>
+      <c r="R20" s="3">
+        <v>71</v>
+      </c>
+      <c r="S20" s="3">
+        <v>4.99</v>
+      </c>
+      <c r="T20" s="3">
+        <v>2</v>
+      </c>
+      <c r="U20" s="3">
+        <v>634</v>
+      </c>
+      <c r="V20" s="3">
+        <v>62.85</v>
+      </c>
+      <c r="W20" s="3">
+        <v>1714190</v>
+      </c>
+      <c r="X20" s="3">
+        <v>169940</v>
+      </c>
+      <c r="Y20" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A21" s="3">
+        <v>3</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="3">
+        <v>2</v>
+      </c>
+      <c r="D21" s="3">
+        <v>80</v>
+      </c>
+      <c r="E21" s="3">
+        <v>5.94</v>
+      </c>
+      <c r="F21" s="3">
+        <v>3</v>
+      </c>
+      <c r="G21" s="3">
+        <v>642</v>
+      </c>
+      <c r="H21" s="3">
+        <v>63.55</v>
+      </c>
+      <c r="I21" s="3">
+        <v>282354</v>
+      </c>
+      <c r="J21" s="3">
+        <v>27950</v>
+      </c>
+      <c r="K21" s="3">
+        <v>0</v>
+      </c>
+      <c r="L21" s="3">
+        <v>0</v>
+      </c>
+      <c r="O21" s="3">
+        <v>3</v>
+      </c>
+      <c r="P21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q21" s="3">
+        <v>1</v>
+      </c>
+      <c r="R21" s="3">
+        <v>91</v>
+      </c>
+      <c r="S21" s="3">
+        <v>4.7699999999999996</v>
+      </c>
+      <c r="T21" s="3">
+        <v>2</v>
+      </c>
+      <c r="U21" s="3">
+        <v>632</v>
+      </c>
+      <c r="V21" s="3">
+        <v>62.85</v>
+      </c>
+      <c r="W21" s="3">
+        <v>1708784</v>
+      </c>
+      <c r="X21" s="3">
+        <v>169943</v>
+      </c>
+      <c r="Y21" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A22" s="3">
+        <v>4</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C22" s="3">
+        <v>2</v>
+      </c>
+      <c r="D22" s="3">
+        <v>66</v>
+      </c>
+      <c r="E22" s="3">
+        <v>4.3600000000000003</v>
+      </c>
+      <c r="F22" s="3">
+        <v>4</v>
+      </c>
+      <c r="G22" s="3">
+        <v>640</v>
+      </c>
+      <c r="H22" s="3">
+        <v>63.47</v>
+      </c>
+      <c r="I22" s="3">
+        <v>281457</v>
+      </c>
+      <c r="J22" s="3">
+        <v>27914</v>
+      </c>
+      <c r="K22" s="3">
+        <v>0</v>
+      </c>
+      <c r="L22" s="3">
+        <v>0</v>
+      </c>
+      <c r="O22" s="3">
+        <v>4</v>
+      </c>
+      <c r="P22" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q22" s="3">
+        <v>2</v>
+      </c>
+      <c r="R22" s="3">
+        <v>126</v>
+      </c>
+      <c r="S22" s="3">
+        <v>6.47</v>
+      </c>
+      <c r="T22" s="3">
+        <v>3</v>
+      </c>
+      <c r="U22" s="3">
+        <v>643</v>
+      </c>
+      <c r="V22" s="3">
+        <v>63.66</v>
+      </c>
+      <c r="W22" s="3">
+        <v>1738550</v>
+      </c>
+      <c r="X22" s="3">
+        <v>172150</v>
+      </c>
+      <c r="Y22" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A23" s="3">
+        <v>5</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="3">
+        <v>2</v>
+      </c>
+      <c r="D23" s="3">
+        <v>40</v>
+      </c>
+      <c r="E23" s="3">
+        <v>3.88</v>
+      </c>
+      <c r="F23" s="3">
+        <v>3</v>
+      </c>
+      <c r="G23" s="3">
+        <v>632</v>
+      </c>
+      <c r="H23" s="3">
+        <v>62.77</v>
+      </c>
+      <c r="I23" s="3">
+        <v>277945</v>
+      </c>
+      <c r="J23" s="3">
+        <v>27606</v>
+      </c>
+      <c r="K23" s="3">
+        <v>0</v>
+      </c>
+      <c r="L23" s="3">
+        <v>0</v>
+      </c>
+      <c r="O23" s="3">
+        <v>5</v>
+      </c>
+      <c r="P23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q23" s="3">
+        <v>1</v>
+      </c>
+      <c r="R23" s="3">
+        <v>21</v>
+      </c>
+      <c r="S23" s="3">
+        <v>3.26</v>
+      </c>
+      <c r="T23" s="3">
+        <v>3</v>
+      </c>
+      <c r="U23" s="3">
+        <v>632</v>
+      </c>
+      <c r="V23" s="3">
+        <v>62.45</v>
+      </c>
+      <c r="W23" s="3">
+        <v>1708790</v>
+      </c>
+      <c r="X23" s="3">
+        <v>168852</v>
+      </c>
+      <c r="Y23" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z23" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A24" s="3">
+        <v>6</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C24" s="3">
+        <v>2</v>
+      </c>
+      <c r="D24" s="3">
+        <v>31</v>
+      </c>
+      <c r="E24" s="3">
+        <v>3.72</v>
+      </c>
+      <c r="F24" s="3">
+        <v>6</v>
+      </c>
+      <c r="G24" s="3">
+        <v>644</v>
+      </c>
+      <c r="H24" s="3">
+        <v>63.81</v>
+      </c>
+      <c r="I24" s="3">
+        <v>283212</v>
+      </c>
+      <c r="J24" s="3">
+        <v>28063</v>
+      </c>
+      <c r="K24" s="3">
+        <v>0</v>
+      </c>
+      <c r="L24" s="3">
+        <v>0</v>
+      </c>
+      <c r="O24" s="3">
+        <v>6</v>
+      </c>
+      <c r="P24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q24" s="3">
+        <v>2</v>
+      </c>
+      <c r="R24" s="3">
+        <v>108</v>
+      </c>
+      <c r="S24" s="3">
+        <v>4.8</v>
+      </c>
+      <c r="T24" s="3">
+        <v>3</v>
+      </c>
+      <c r="U24" s="3">
+        <v>634</v>
+      </c>
+      <c r="V24" s="3">
+        <v>62.94</v>
+      </c>
+      <c r="W24" s="3">
+        <v>1714189</v>
+      </c>
+      <c r="X24" s="3">
+        <v>170193</v>
+      </c>
+      <c r="Y24" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z24" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A25" s="3">
+        <v>7</v>
+      </c>
+      <c r="B25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C25" s="3">
+        <v>2</v>
+      </c>
+      <c r="D25" s="3">
+        <v>53</v>
+      </c>
+      <c r="E25" s="3">
+        <v>4.66</v>
+      </c>
+      <c r="F25" s="3">
+        <v>2</v>
+      </c>
+      <c r="G25" s="3">
+        <v>642</v>
+      </c>
+      <c r="H25" s="3">
+        <v>63.7</v>
+      </c>
+      <c r="I25" s="3">
+        <v>282344</v>
+      </c>
+      <c r="J25" s="3">
+        <v>28015</v>
+      </c>
+      <c r="K25" s="3">
+        <v>0</v>
+      </c>
+      <c r="L25" s="3">
+        <v>0</v>
+      </c>
+      <c r="O25" s="3">
+        <v>7</v>
+      </c>
+      <c r="P25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q25" s="3">
+        <v>2</v>
+      </c>
+      <c r="R25" s="3">
+        <v>98</v>
+      </c>
+      <c r="S25" s="3">
+        <v>5.89</v>
+      </c>
+      <c r="T25" s="3">
+        <v>2</v>
+      </c>
+      <c r="U25" s="3">
+        <v>632</v>
+      </c>
+      <c r="V25" s="3">
+        <v>62.66</v>
+      </c>
+      <c r="W25" s="3">
+        <v>1708786</v>
+      </c>
+      <c r="X25" s="3">
+        <v>169421</v>
+      </c>
+      <c r="Y25" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z25" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A26" s="3">
+        <v>8</v>
+      </c>
+      <c r="B26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C26" s="3">
+        <v>2</v>
+      </c>
+      <c r="D26" s="3">
+        <v>28</v>
+      </c>
+      <c r="E26" s="3">
+        <v>3.69</v>
+      </c>
+      <c r="F26" s="3">
+        <v>4</v>
+      </c>
+      <c r="G26" s="3">
+        <v>642</v>
+      </c>
+      <c r="H26" s="3">
+        <v>63.84</v>
+      </c>
+      <c r="I26" s="3">
+        <v>282350</v>
+      </c>
+      <c r="J26" s="3">
+        <v>28077</v>
+      </c>
+      <c r="K26" s="3">
+        <v>0</v>
+      </c>
+      <c r="L26" s="3">
+        <v>0</v>
+      </c>
+      <c r="O26" s="3">
+        <v>8</v>
+      </c>
+      <c r="P26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q26" s="3">
+        <v>2</v>
+      </c>
+      <c r="R26" s="3">
+        <v>10</v>
+      </c>
+      <c r="S26" s="3">
+        <v>2.94</v>
+      </c>
+      <c r="T26" s="3">
+        <v>3</v>
+      </c>
+      <c r="U26" s="3">
+        <v>639</v>
+      </c>
+      <c r="V26" s="3">
+        <v>63.5</v>
+      </c>
+      <c r="W26" s="3">
+        <v>1727704</v>
+      </c>
+      <c r="X26" s="3">
+        <v>171705</v>
+      </c>
+      <c r="Y26" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z26" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="27" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A27" s="3">
+        <v>9</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C27" s="3">
+        <v>2</v>
+      </c>
+      <c r="D27" s="3">
+        <v>62</v>
+      </c>
+      <c r="E27" s="3">
+        <v>4.57</v>
+      </c>
+      <c r="F27" s="3">
+        <v>2</v>
+      </c>
+      <c r="G27" s="3">
+        <v>640</v>
+      </c>
+      <c r="H27" s="3">
+        <v>63.62</v>
+      </c>
+      <c r="I27" s="3">
+        <v>281461</v>
+      </c>
+      <c r="J27" s="3">
+        <v>27981</v>
+      </c>
+      <c r="K27" s="3">
+        <v>0</v>
+      </c>
+      <c r="L27" s="3">
+        <v>0</v>
+      </c>
+      <c r="O27" s="3">
+        <v>9</v>
+      </c>
+      <c r="P27" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q27" s="3">
+        <v>2</v>
+      </c>
+      <c r="R27" s="3">
+        <v>24</v>
+      </c>
+      <c r="S27" s="3">
+        <v>3.37</v>
+      </c>
+      <c r="T27" s="3">
+        <v>3</v>
+      </c>
+      <c r="U27" s="3">
+        <v>636</v>
+      </c>
+      <c r="V27" s="3">
+        <v>63.02</v>
+      </c>
+      <c r="W27" s="3">
+        <v>1719608</v>
+      </c>
+      <c r="X27" s="3">
+        <v>170393</v>
+      </c>
+      <c r="Y27" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z27" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A28" s="3">
+        <v>10</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C28" s="3">
+        <v>2</v>
+      </c>
+      <c r="D28" s="3">
+        <v>29</v>
+      </c>
+      <c r="E28" s="3">
+        <v>3.63</v>
+      </c>
+      <c r="F28" s="3">
+        <v>29</v>
+      </c>
+      <c r="G28" s="3">
+        <v>636</v>
+      </c>
+      <c r="H28" s="3">
+        <v>63.05</v>
+      </c>
+      <c r="I28" s="3">
+        <v>279711</v>
+      </c>
+      <c r="J28" s="3">
+        <v>27732</v>
+      </c>
+      <c r="K28" s="3">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3">
+        <v>0</v>
+      </c>
+      <c r="O28" s="3">
+        <v>10</v>
+      </c>
+      <c r="P28" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q28" s="3">
+        <v>2</v>
+      </c>
+      <c r="R28" s="3">
+        <v>119</v>
+      </c>
+      <c r="S28" s="3">
+        <v>5.47</v>
+      </c>
+      <c r="T28" s="3">
+        <v>3</v>
+      </c>
+      <c r="U28" s="3">
+        <v>624</v>
+      </c>
+      <c r="V28" s="3">
+        <v>62.05</v>
+      </c>
+      <c r="W28" s="3">
+        <v>1687148</v>
+      </c>
+      <c r="X28" s="3">
+        <v>167775</v>
+      </c>
+      <c r="Y28" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z28" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A29" s="3">
+        <v>11</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C29" s="3">
+        <v>2</v>
+      </c>
+      <c r="D29" s="3">
+        <v>43</v>
+      </c>
+      <c r="E29" s="3">
+        <v>4.04</v>
+      </c>
+      <c r="F29" s="3">
+        <v>4</v>
+      </c>
+      <c r="G29" s="3">
+        <v>627</v>
+      </c>
+      <c r="H29" s="3">
+        <v>62.22</v>
+      </c>
+      <c r="I29" s="3">
+        <v>275756</v>
+      </c>
+      <c r="J29" s="3">
+        <v>27367</v>
+      </c>
+      <c r="K29" s="3">
+        <v>0</v>
+      </c>
+      <c r="L29" s="3">
+        <v>0</v>
+      </c>
+      <c r="O29" s="3">
+        <v>11</v>
+      </c>
+      <c r="P29" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q29" s="3">
+        <v>2</v>
+      </c>
+      <c r="R29" s="3">
+        <v>49</v>
+      </c>
+      <c r="S29" s="3">
+        <v>3.89</v>
+      </c>
+      <c r="T29" s="3">
+        <v>3</v>
+      </c>
+      <c r="U29" s="3">
+        <v>635</v>
+      </c>
+      <c r="V29" s="3">
+        <v>63.02</v>
+      </c>
+      <c r="W29" s="3">
+        <v>1716909</v>
+      </c>
+      <c r="X29" s="3">
+        <v>170412</v>
+      </c>
+      <c r="Y29" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z29" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A30" s="3">
+        <v>12</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C30" s="3">
+        <v>2</v>
+      </c>
+      <c r="D30" s="3">
+        <v>50</v>
+      </c>
+      <c r="E30" s="3">
+        <v>4.6500000000000004</v>
+      </c>
+      <c r="F30" s="3">
+        <v>3</v>
+      </c>
+      <c r="G30" s="3">
+        <v>639</v>
+      </c>
+      <c r="H30" s="3">
+        <v>63.32</v>
+      </c>
+      <c r="I30" s="3">
+        <v>281025</v>
+      </c>
+      <c r="J30" s="3">
+        <v>27849</v>
+      </c>
+      <c r="K30" s="3">
+        <v>0</v>
+      </c>
+      <c r="L30" s="3">
+        <v>0</v>
+      </c>
+      <c r="O30" s="3">
+        <v>12</v>
+      </c>
+      <c r="P30" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q30" s="3">
+        <v>1</v>
+      </c>
+      <c r="R30" s="3">
+        <v>55</v>
+      </c>
+      <c r="S30" s="3">
+        <v>4.5599999999999996</v>
+      </c>
+      <c r="T30" s="3">
+        <v>2</v>
+      </c>
+      <c r="U30" s="3">
+        <v>636</v>
+      </c>
+      <c r="V30" s="3">
+        <v>63.25</v>
+      </c>
+      <c r="W30" s="3">
+        <v>1719591</v>
+      </c>
+      <c r="X30" s="3">
+        <v>171035</v>
+      </c>
+      <c r="Y30" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z30" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="8"/>
+      <c r="I33" s="8"/>
+      <c r="J33" s="8"/>
+      <c r="K33" s="8"/>
+      <c r="L33" s="8"/>
+      <c r="O33" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+    </row>
+    <row r="34" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A34" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C34" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D34" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E34" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F34" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="G34" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="H34" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="I34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="J34" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="K34" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="L34" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O34" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="P34" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q34" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="R34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="S34" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="T34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="U34" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="V34" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="W34" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="X34" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="Y34" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="Z34" s="5" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="35" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A35" s="3">
+        <v>1</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C35" s="3">
+        <v>1</v>
+      </c>
+      <c r="D35" s="3">
+        <v>43</v>
+      </c>
+      <c r="E35" s="3">
+        <v>5.17</v>
+      </c>
+      <c r="F35" s="3">
+        <v>2</v>
+      </c>
+      <c r="G35" s="3">
+        <v>1291</v>
+      </c>
+      <c r="H35" s="3">
+        <v>128.04</v>
+      </c>
+      <c r="I35" s="3">
+        <v>567761</v>
+      </c>
+      <c r="J35" s="3">
+        <v>56314</v>
+      </c>
+      <c r="K35" s="3">
+        <v>0</v>
+      </c>
+      <c r="L35" s="3">
+        <v>0</v>
+      </c>
+      <c r="O35" s="3">
+        <v>1</v>
+      </c>
+      <c r="P35" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q35" s="3">
+        <v>2</v>
+      </c>
+      <c r="R35" s="3">
+        <v>35</v>
+      </c>
+      <c r="S35" s="3">
+        <v>3.47</v>
+      </c>
+      <c r="T35" s="3">
+        <v>18</v>
+      </c>
+      <c r="U35" s="3">
+        <v>1288</v>
+      </c>
+      <c r="V35" s="3">
+        <v>127.38</v>
+      </c>
+      <c r="W35" s="3">
+        <v>3482463</v>
+      </c>
+      <c r="X35" s="3">
+        <v>344423</v>
+      </c>
+      <c r="Y35" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z35" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="36" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A36" s="3">
+        <v>2</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C36" s="3">
+        <v>2</v>
+      </c>
+      <c r="D36" s="3">
+        <v>48</v>
+      </c>
+      <c r="E36" s="3">
+        <v>4.04</v>
+      </c>
+      <c r="F36" s="3">
+        <v>2</v>
+      </c>
+      <c r="G36" s="3">
+        <v>1272</v>
+      </c>
+      <c r="H36" s="3">
+        <v>126.14</v>
+      </c>
+      <c r="I36" s="3">
+        <v>559434</v>
+      </c>
+      <c r="J36" s="3">
+        <v>55477</v>
+      </c>
+      <c r="K36" s="3">
+        <v>0</v>
+      </c>
+      <c r="L36" s="3">
+        <v>0</v>
+      </c>
+      <c r="O36" s="3">
+        <v>2</v>
+      </c>
+      <c r="P36" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q36" s="3">
+        <v>2</v>
+      </c>
+      <c r="R36" s="3">
+        <v>120</v>
+      </c>
+      <c r="S36" s="3">
+        <v>5.79</v>
+      </c>
+      <c r="T36" s="3">
+        <v>2</v>
+      </c>
+      <c r="U36" s="3">
+        <v>1261</v>
+      </c>
+      <c r="V36" s="3">
+        <v>124.87</v>
+      </c>
+      <c r="W36" s="3">
+        <v>3409447</v>
+      </c>
+      <c r="X36" s="3">
+        <v>337635</v>
+      </c>
+      <c r="Y36" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z36" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A37" s="3">
+        <v>3</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C37" s="3">
+        <v>2</v>
+      </c>
+      <c r="D37" s="3">
+        <v>41</v>
+      </c>
+      <c r="E37" s="3">
+        <v>4.66</v>
+      </c>
+      <c r="F37" s="3">
+        <v>3</v>
+      </c>
+      <c r="G37" s="3">
+        <v>1283</v>
+      </c>
+      <c r="H37" s="3">
+        <v>127.35</v>
+      </c>
+      <c r="I37" s="3">
+        <v>564221</v>
+      </c>
+      <c r="J37" s="3">
+        <v>56007</v>
+      </c>
+      <c r="K37" s="3">
+        <v>0</v>
+      </c>
+      <c r="L37" s="3">
+        <v>0</v>
+      </c>
+      <c r="O37" s="3">
+        <v>3</v>
+      </c>
+      <c r="P37" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q37" s="3">
+        <v>2</v>
+      </c>
+      <c r="R37" s="3">
+        <v>52</v>
+      </c>
+      <c r="S37" s="3">
+        <v>5.15</v>
+      </c>
+      <c r="T37" s="3">
+        <v>2</v>
+      </c>
+      <c r="U37" s="3">
+        <v>1270</v>
+      </c>
+      <c r="V37" s="3">
+        <v>124.25</v>
+      </c>
+      <c r="W37" s="3">
+        <v>3433796</v>
+      </c>
+      <c r="X37" s="3">
+        <v>335954</v>
+      </c>
+      <c r="Y37" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z37" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A38" s="3">
+        <v>4</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C38" s="3">
+        <v>2</v>
+      </c>
+      <c r="D38" s="3">
+        <v>167</v>
+      </c>
+      <c r="E38" s="3">
+        <v>7.57</v>
+      </c>
+      <c r="F38" s="3">
+        <v>3</v>
+      </c>
+      <c r="G38" s="3">
+        <v>1271</v>
+      </c>
+      <c r="H38" s="3">
+        <v>126.15</v>
+      </c>
+      <c r="I38" s="3">
+        <v>558928</v>
+      </c>
+      <c r="J38" s="3">
+        <v>55476</v>
+      </c>
+      <c r="K38" s="3">
+        <v>0</v>
+      </c>
+      <c r="L38" s="3">
+        <v>0</v>
+      </c>
+      <c r="O38" s="3">
+        <v>4</v>
+      </c>
+      <c r="P38" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q38" s="3">
+        <v>1</v>
+      </c>
+      <c r="R38" s="3">
+        <v>56</v>
+      </c>
+      <c r="S38" s="3">
+        <v>4.13</v>
+      </c>
+      <c r="T38" s="3">
+        <v>3</v>
+      </c>
+      <c r="U38" s="3">
+        <v>1289</v>
+      </c>
+      <c r="V38" s="3">
+        <v>126.38</v>
+      </c>
+      <c r="W38" s="3">
+        <v>3485172</v>
+      </c>
+      <c r="X38" s="3">
+        <v>341717</v>
+      </c>
+      <c r="Y38" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z38" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A39" s="3">
+        <v>5</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C39" s="3">
+        <v>2</v>
+      </c>
+      <c r="D39" s="3">
+        <v>57</v>
+      </c>
+      <c r="E39" s="3">
+        <v>5.07</v>
+      </c>
+      <c r="F39" s="3">
+        <v>3</v>
+      </c>
+      <c r="G39" s="3">
+        <v>1273</v>
+      </c>
+      <c r="H39" s="3">
+        <v>126.31</v>
+      </c>
+      <c r="I39" s="3">
+        <v>559834</v>
+      </c>
+      <c r="J39" s="3">
+        <v>55550</v>
+      </c>
+      <c r="K39" s="3">
+        <v>0</v>
+      </c>
+      <c r="L39" s="3">
+        <v>0</v>
+      </c>
+      <c r="O39" s="3">
+        <v>5</v>
+      </c>
+      <c r="P39" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q39" s="3">
+        <v>1</v>
+      </c>
+      <c r="R39" s="3">
+        <v>173</v>
+      </c>
+      <c r="S39" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="T39" s="3">
+        <v>2</v>
+      </c>
+      <c r="U39" s="3">
+        <v>1260</v>
+      </c>
+      <c r="V39" s="3">
+        <v>125.27</v>
+      </c>
+      <c r="W39" s="3">
+        <v>3406761</v>
+      </c>
+      <c r="X39" s="3">
+        <v>338711</v>
+      </c>
+      <c r="Y39" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z39" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A40" s="3">
+        <v>6</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C40" s="3">
+        <v>2</v>
+      </c>
+      <c r="D40" s="3">
+        <v>109</v>
+      </c>
+      <c r="E40" s="3">
+        <v>6.66</v>
+      </c>
+      <c r="F40" s="3">
+        <v>4</v>
+      </c>
+      <c r="G40" s="3">
+        <v>1269</v>
+      </c>
+      <c r="H40" s="3">
+        <v>125.96</v>
+      </c>
+      <c r="I40" s="3">
+        <v>558079</v>
+      </c>
+      <c r="J40" s="3">
+        <v>55397</v>
+      </c>
+      <c r="K40" s="3">
+        <v>0</v>
+      </c>
+      <c r="L40" s="3">
+        <v>0</v>
+      </c>
+      <c r="O40" s="3">
+        <v>6</v>
+      </c>
+      <c r="P40" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q40" s="3">
+        <v>1</v>
+      </c>
+      <c r="R40" s="3">
+        <v>93</v>
+      </c>
+      <c r="S40" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="T40" s="3">
+        <v>3</v>
+      </c>
+      <c r="U40" s="3">
+        <v>1274</v>
+      </c>
+      <c r="V40" s="3">
+        <v>126.53</v>
+      </c>
+      <c r="W40" s="3">
+        <v>3444565</v>
+      </c>
+      <c r="X40" s="3">
+        <v>342130</v>
+      </c>
+      <c r="Y40" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z40" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="41" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A41" s="3">
+        <v>7</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C41" s="3">
+        <v>2</v>
+      </c>
+      <c r="D41" s="3">
+        <v>96</v>
+      </c>
+      <c r="E41" s="3">
+        <v>5.53</v>
+      </c>
+      <c r="F41" s="3">
+        <v>3</v>
+      </c>
+      <c r="G41" s="3">
+        <v>1277</v>
+      </c>
+      <c r="H41" s="3">
+        <v>126.48</v>
+      </c>
+      <c r="I41" s="3">
+        <v>561595</v>
+      </c>
+      <c r="J41" s="3">
+        <v>55625</v>
+      </c>
+      <c r="K41" s="3">
+        <v>0</v>
+      </c>
+      <c r="L41" s="3">
+        <v>0</v>
+      </c>
+      <c r="O41" s="3">
+        <v>7</v>
+      </c>
+      <c r="P41" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q41" s="3">
+        <v>2</v>
+      </c>
+      <c r="R41" s="3">
+        <v>141</v>
+      </c>
+      <c r="S41" s="3">
+        <v>7.81</v>
+      </c>
+      <c r="T41" s="3">
+        <v>5</v>
+      </c>
+      <c r="U41" s="3">
+        <v>1287</v>
+      </c>
+      <c r="V41" s="3">
+        <v>127.62</v>
+      </c>
+      <c r="W41" s="3">
+        <v>3479750</v>
+      </c>
+      <c r="X41" s="3">
+        <v>345076</v>
+      </c>
+      <c r="Y41" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z41" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="42" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A42" s="3">
+        <v>8</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C42" s="3">
+        <v>2</v>
+      </c>
+      <c r="D42" s="3">
+        <v>109</v>
+      </c>
+      <c r="E42" s="3">
+        <v>6.44</v>
+      </c>
+      <c r="F42" s="3">
+        <v>2</v>
+      </c>
+      <c r="G42" s="3">
+        <v>1287</v>
+      </c>
+      <c r="H42" s="3">
+        <v>127.37</v>
+      </c>
+      <c r="I42" s="3">
+        <v>565991</v>
+      </c>
+      <c r="J42" s="3">
+        <v>56016</v>
+      </c>
+      <c r="K42" s="3">
+        <v>0</v>
+      </c>
+      <c r="L42" s="3">
+        <v>0</v>
+      </c>
+      <c r="O42" s="3">
+        <v>8</v>
+      </c>
+      <c r="P42" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q42" s="3">
+        <v>1</v>
+      </c>
+      <c r="R42" s="3">
+        <v>160</v>
+      </c>
+      <c r="S42" s="3">
+        <v>10.15</v>
+      </c>
+      <c r="T42" s="3">
+        <v>3</v>
+      </c>
+      <c r="U42" s="3">
+        <v>1277</v>
+      </c>
+      <c r="V42" s="3">
+        <v>126.68</v>
+      </c>
+      <c r="W42" s="3">
+        <v>3452736</v>
+      </c>
+      <c r="X42" s="3">
+        <v>342533</v>
+      </c>
+      <c r="Y42" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z42" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A43" s="3">
+        <v>9</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C43" s="3">
+        <v>1</v>
+      </c>
+      <c r="D43" s="3">
+        <v>107</v>
+      </c>
+      <c r="E43" s="3">
+        <v>6.86</v>
+      </c>
+      <c r="F43" s="3">
+        <v>4</v>
+      </c>
+      <c r="G43" s="3">
+        <v>1261</v>
+      </c>
+      <c r="H43" s="3">
+        <v>124.93</v>
+      </c>
+      <c r="I43" s="3">
+        <v>554576</v>
+      </c>
+      <c r="J43" s="3">
+        <v>54946</v>
+      </c>
+      <c r="K43" s="3">
+        <v>0</v>
+      </c>
+      <c r="L43" s="3">
+        <v>0</v>
+      </c>
+      <c r="O43" s="3">
+        <v>9</v>
+      </c>
+      <c r="P43" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q43" s="3">
+        <v>1</v>
+      </c>
+      <c r="R43" s="3">
+        <v>111</v>
+      </c>
+      <c r="S43" s="3">
+        <v>5.2</v>
+      </c>
+      <c r="T43" s="3">
+        <v>3</v>
+      </c>
+      <c r="U43" s="3">
+        <v>1281</v>
+      </c>
+      <c r="V43" s="3">
+        <v>127.03</v>
+      </c>
+      <c r="W43" s="3">
+        <v>3463559</v>
+      </c>
+      <c r="X43" s="3">
+        <v>343470</v>
+      </c>
+      <c r="Y43" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z43" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A44" s="3">
+        <v>10</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C44" s="3">
+        <v>2</v>
+      </c>
+      <c r="D44" s="3">
+        <v>78</v>
+      </c>
+      <c r="E44" s="3">
+        <v>5.52</v>
+      </c>
+      <c r="F44" s="3">
+        <v>3</v>
+      </c>
+      <c r="G44" s="3">
+        <v>1271</v>
+      </c>
+      <c r="H44" s="3">
+        <v>125.96</v>
+      </c>
+      <c r="I44" s="3">
+        <v>558932</v>
+      </c>
+      <c r="J44" s="3">
+        <v>55394</v>
+      </c>
+      <c r="K44" s="3">
+        <v>0</v>
+      </c>
+      <c r="L44" s="3">
+        <v>0</v>
+      </c>
+      <c r="O44" s="3">
+        <v>10</v>
+      </c>
+      <c r="P44" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q44" s="3">
+        <v>2</v>
+      </c>
+      <c r="R44" s="3">
+        <v>177</v>
+      </c>
+      <c r="S44" s="3">
+        <v>11.73</v>
+      </c>
+      <c r="T44" s="3">
+        <v>2</v>
+      </c>
+      <c r="U44" s="3">
+        <v>1257</v>
+      </c>
+      <c r="V44" s="3">
+        <v>124.83</v>
+      </c>
+      <c r="W44" s="3">
+        <v>3398653</v>
+      </c>
+      <c r="X44" s="3">
+        <v>337536</v>
+      </c>
+      <c r="Y44" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z44" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="45" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A45" s="3">
+        <v>11</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C45" s="3">
+        <v>2</v>
+      </c>
+      <c r="D45" s="3">
+        <v>75</v>
+      </c>
+      <c r="E45" s="3">
+        <v>5.53</v>
+      </c>
+      <c r="F45" s="3">
+        <v>29</v>
+      </c>
+      <c r="G45" s="3">
+        <v>1276</v>
+      </c>
+      <c r="H45" s="3">
+        <v>126.33</v>
+      </c>
+      <c r="I45" s="3">
+        <v>561178</v>
+      </c>
+      <c r="J45" s="3">
+        <v>55562</v>
+      </c>
+      <c r="K45" s="3">
+        <v>0</v>
+      </c>
+      <c r="L45" s="3">
+        <v>0</v>
+      </c>
+      <c r="O45" s="3">
+        <v>11</v>
+      </c>
+      <c r="P45" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q45" s="3">
+        <v>2</v>
+      </c>
+      <c r="R45" s="3">
+        <v>56</v>
+      </c>
+      <c r="S45" s="3">
+        <v>4.6900000000000004</v>
+      </c>
+      <c r="T45" s="3">
+        <v>2</v>
+      </c>
+      <c r="U45" s="3">
+        <v>1263</v>
+      </c>
+      <c r="V45" s="3">
+        <v>125.13</v>
+      </c>
+      <c r="W45" s="3">
+        <v>3414854</v>
+      </c>
+      <c r="X45" s="3">
+        <v>338338</v>
+      </c>
+      <c r="Y45" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z45" s="3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:26" x14ac:dyDescent="0.25">
+      <c r="A46" s="3">
+        <v>12</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="3">
+        <v>2</v>
+      </c>
+      <c r="D46" s="3">
+        <v>138</v>
+      </c>
+      <c r="E46" s="3">
+        <v>5.5</v>
+      </c>
+      <c r="F46" s="3">
+        <v>6</v>
+      </c>
+      <c r="G46" s="3">
+        <v>1281</v>
+      </c>
+      <c r="H46" s="3">
+        <v>126.69</v>
+      </c>
+      <c r="I46" s="3">
+        <v>563377</v>
+      </c>
+      <c r="J46" s="3">
+        <v>55719</v>
+      </c>
+      <c r="K46" s="3">
+        <v>0</v>
+      </c>
+      <c r="L46" s="3">
+        <v>0</v>
+      </c>
+      <c r="O46" s="3">
+        <v>12</v>
+      </c>
+      <c r="P46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q46" s="3">
+        <v>2</v>
+      </c>
+      <c r="R46" s="3">
+        <v>103</v>
+      </c>
+      <c r="S46" s="3">
+        <v>5.72</v>
+      </c>
+      <c r="T46" s="3">
+        <v>3</v>
+      </c>
+      <c r="U46" s="3">
+        <v>1268</v>
+      </c>
+      <c r="V46" s="3">
+        <v>125.95</v>
+      </c>
+      <c r="W46" s="3">
+        <v>3428383</v>
+      </c>
+      <c r="X46" s="3">
+        <v>340556</v>
+      </c>
+      <c r="Y46" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z46" s="3">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="8">
+    <mergeCell ref="A33:L33"/>
+    <mergeCell ref="O33:Z33"/>
+    <mergeCell ref="A1:L1"/>
+    <mergeCell ref="O1:Z1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="O2:Z2"/>
+    <mergeCell ref="A17:L17"/>
+    <mergeCell ref="O17:Z17"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>